<commit_message>
get_profile_all() in CostData largely completed. lots of exception handling required. Some finessing required. All tests passing
</commit_message>
<xml_diff>
--- a/tests/resources/cost_test_master_4_2018.xlsx
+++ b/tests/resources/cost_test_master_4_2018.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="418">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -1285,7 +1285,7 @@
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1349,12 +1349,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1440,7 +1434,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1524,11 +1518,11 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B365" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B344" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A365" activeCellId="0" sqref="A365"/>
-      <selection pane="bottomRight" activeCell="I382" activeCellId="0" sqref="I382"/>
+      <selection pane="bottomLeft" activeCell="A344" activeCellId="0" sqref="A344"/>
+      <selection pane="bottomRight" activeCell="F371" activeCellId="0" sqref="F371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6617,7 +6611,9 @@
         <v>410</v>
       </c>
       <c r="B374" s="8"/>
-      <c r="C374" s="8"/>
+      <c r="C374" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="D374" s="8" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
exception handling for single project cost profiles
</commit_message>
<xml_diff>
--- a/tests/resources/cost_test_master_4_2018.xlsx
+++ b/tests/resources/cost_test_master_4_2018.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="418">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">Columbia</t>
   </si>
   <si>
+    <t xml:space="preserve">Apollo 11</t>
+  </si>
+  <si>
     <t xml:space="preserve">Project stage</t>
   </si>
   <si>
@@ -122,9 +125,6 @@
   </si>
   <si>
     <t xml:space="preserve">nail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green lumber fallacy</t>
   </si>
   <si>
     <t xml:space="preserve">Please provide details of any formal arrangement with HMT regarding Business cases, that are outside the classical model</t>
@@ -1518,11 +1518,11 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B344" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B358" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A344" activeCellId="0" sqref="A344"/>
-      <selection pane="bottomRight" activeCell="F371" activeCellId="0" sqref="F371"/>
+      <selection pane="bottomLeft" activeCell="A358" activeCellId="0" sqref="A358"/>
+      <selection pane="bottomRight" activeCell="G369" activeCellId="0" sqref="G369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1546,73 +1546,89 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>40875</v>
@@ -1623,115 +1639,133 @@
       <c r="D7" s="4" t="n">
         <v>41852</v>
       </c>
+      <c r="E7" s="4" t="n">
+        <v>42387</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
       <c r="D11" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
       <c r="D12" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
       <c r="D13" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1740,6 +1774,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -1754,6 +1789,9 @@
       <c r="D19" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="E19" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
@@ -1768,6 +1806,9 @@
       <c r="D20" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="E20" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -1775,6 +1816,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
@@ -1782,19 +1824,23 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1803,19 +1849,23 @@
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1829,6 +1879,9 @@
       <c r="D26" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="E26" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
@@ -1836,10 +1889,13 @@
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1851,7 +1907,10 @@
         <v>49</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1865,6 +1924,9 @@
       <c r="D29" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="E29" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
@@ -1877,6 +1939,9 @@
       <c r="D30" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="E30" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
@@ -1884,6 +1949,7 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="3"/>
+      <c r="E31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
@@ -1891,6 +1957,7 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="3"/>
+      <c r="E32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
@@ -1898,10 +1965,13 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>20</v>
+      <c r="E33" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1913,19 +1983,23 @@
       <c r="D34" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="E34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>20</v>
+      <c r="E35" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1938,6 +2012,9 @@
       <c r="C36" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="E36" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
@@ -1949,6 +2026,9 @@
       <c r="C37" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="E37" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
@@ -1958,6 +2038,9 @@
       <c r="C38" s="1" t="n">
         <v>2010</v>
       </c>
+      <c r="E38" s="1" t="n">
+        <v>2010</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
@@ -1965,16 +2048,20 @@
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="3"/>
+      <c r="E39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1983,6 +2070,7 @@
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="3"/>
+      <c r="E41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
@@ -1997,6 +2085,9 @@
       <c r="D42" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="E42" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
@@ -2009,6 +2100,9 @@
       <c r="D43" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="E43" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
@@ -2018,6 +2112,9 @@
       <c r="C44" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E44" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
@@ -2027,6 +2124,9 @@
       <c r="C45" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E45" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
@@ -2036,6 +2136,9 @@
       <c r="C46" s="1" t="n">
         <v>0.11</v>
       </c>
+      <c r="E46" s="1" t="n">
+        <v>0.11</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
@@ -2045,6 +2148,9 @@
       <c r="C47" s="1" t="n">
         <v>609</v>
       </c>
+      <c r="E47" s="1" t="n">
+        <v>609</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
@@ -2056,6 +2162,9 @@
       <c r="C48" s="1" t="n">
         <v>2952</v>
       </c>
+      <c r="E48" s="1" t="n">
+        <v>2952</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
@@ -2065,6 +2174,9 @@
       <c r="C49" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="E49" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
@@ -2079,6 +2191,9 @@
       <c r="D50" s="2" t="n">
         <v>0.38</v>
       </c>
+      <c r="E50" s="1" t="n">
+        <v>1.52</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
@@ -2093,6 +2208,9 @@
       <c r="D51" s="1" t="n">
         <v>747.7</v>
       </c>
+      <c r="E51" s="1" t="n">
+        <v>4648.8</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
@@ -2107,6 +2225,9 @@
       <c r="D52" s="1" t="n">
         <v>682.16</v>
       </c>
+      <c r="E52" s="1" t="n">
+        <v>5692.07</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
@@ -2121,6 +2242,9 @@
       <c r="D53" s="1" t="n">
         <v>63.06</v>
       </c>
+      <c r="E53" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
@@ -2135,6 +2259,9 @@
       <c r="D54" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E54" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
@@ -2149,6 +2276,9 @@
       <c r="D55" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E55" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
@@ -2163,6 +2293,9 @@
       <c r="D56" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E56" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
@@ -2177,6 +2310,9 @@
       <c r="D57" s="1" t="n">
         <v>63.06</v>
       </c>
+      <c r="E57" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
@@ -2191,6 +2327,9 @@
       <c r="D58" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E58" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
@@ -2205,6 +2344,9 @@
       <c r="D59" s="1" t="n">
         <v>63.02</v>
       </c>
+      <c r="E59" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
@@ -2219,6 +2361,9 @@
       <c r="D60" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E60" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
@@ -2233,6 +2378,9 @@
       <c r="D61" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E61" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
@@ -2247,6 +2395,9 @@
       <c r="D62" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E62" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
@@ -2261,6 +2412,9 @@
       <c r="D63" s="1" t="n">
         <v>63.02</v>
       </c>
+      <c r="E63" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
@@ -2275,6 +2429,9 @@
       <c r="D64" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E64" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
@@ -2289,6 +2446,9 @@
       <c r="D65" s="1" t="n">
         <v>36.22</v>
       </c>
+      <c r="E65" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
@@ -2303,6 +2463,9 @@
       <c r="D66" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E66" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
@@ -2317,6 +2480,9 @@
       <c r="D67" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E67" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
@@ -2331,6 +2497,9 @@
       <c r="D68" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E68" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
@@ -2345,6 +2514,9 @@
       <c r="D69" s="1" t="n">
         <v>36.22</v>
       </c>
+      <c r="E69" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
@@ -2359,6 +2531,9 @@
       <c r="D70" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E70" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
@@ -2373,6 +2548,9 @@
       <c r="D71" s="1" t="n">
         <v>36.22</v>
       </c>
+      <c r="E71" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
@@ -2387,6 +2565,9 @@
       <c r="D72" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E72" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
@@ -2401,6 +2582,9 @@
       <c r="D73" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E73" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
@@ -2415,6 +2599,9 @@
       <c r="D74" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E74" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
@@ -2429,6 +2616,9 @@
       <c r="D75" s="1" t="n">
         <v>36.22</v>
       </c>
+      <c r="E75" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
@@ -2443,6 +2633,9 @@
       <c r="D76" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E76" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
@@ -2457,6 +2650,9 @@
       <c r="D77" s="1" t="n">
         <v>33.42</v>
       </c>
+      <c r="E77" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
@@ -2471,6 +2667,9 @@
       <c r="D78" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E78" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
@@ -2485,6 +2684,9 @@
       <c r="D79" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E79" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
@@ -2499,6 +2701,9 @@
       <c r="D80" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E80" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
@@ -2513,6 +2718,9 @@
       <c r="D81" s="1" t="n">
         <v>33.42</v>
       </c>
+      <c r="E81" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
@@ -2527,6 +2735,9 @@
       <c r="D82" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E82" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
@@ -2541,6 +2752,9 @@
       <c r="D83" s="1" t="n">
         <v>33.42</v>
       </c>
+      <c r="E83" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
@@ -2555,6 +2769,9 @@
       <c r="D84" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E84" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
@@ -2569,6 +2786,9 @@
       <c r="D85" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E85" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
@@ -2583,6 +2803,9 @@
       <c r="D86" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E86" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
@@ -2597,6 +2820,9 @@
       <c r="D87" s="1" t="n">
         <v>33.42</v>
       </c>
+      <c r="E87" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
@@ -2611,6 +2837,9 @@
       <c r="D88" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E88" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
@@ -2625,6 +2854,9 @@
       <c r="D89" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E89" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
@@ -2639,6 +2871,9 @@
       <c r="D90" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E90" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
@@ -2653,6 +2888,9 @@
       <c r="D91" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E91" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
@@ -2667,6 +2905,9 @@
       <c r="D92" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E92" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
@@ -2681,6 +2922,9 @@
       <c r="D93" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E93" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
@@ -2695,6 +2939,9 @@
       <c r="D94" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E94" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
@@ -2709,6 +2956,9 @@
       <c r="D95" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E95" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
@@ -2723,6 +2973,9 @@
       <c r="D96" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E96" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
@@ -2737,6 +2990,9 @@
       <c r="D97" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E97" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
@@ -2751,6 +3007,9 @@
       <c r="D98" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E98" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
@@ -2765,6 +3024,9 @@
       <c r="D99" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E99" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
@@ -2779,6 +3041,9 @@
       <c r="D100" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E100" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
@@ -2793,6 +3058,9 @@
       <c r="D101" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E101" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
@@ -2807,6 +3075,9 @@
       <c r="D102" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E102" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
@@ -2821,6 +3092,9 @@
       <c r="D103" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E103" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
@@ -2835,6 +3109,9 @@
       <c r="D104" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E104" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
@@ -2849,6 +3126,9 @@
       <c r="D105" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E105" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
@@ -2863,6 +3143,9 @@
       <c r="D106" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E106" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
@@ -2877,6 +3160,9 @@
       <c r="D107" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E107" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
@@ -2891,6 +3177,9 @@
       <c r="D108" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E108" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
@@ -2905,6 +3194,9 @@
       <c r="D109" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E109" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
@@ -2919,6 +3211,9 @@
       <c r="D110" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E110" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
@@ -2933,6 +3228,9 @@
       <c r="D111" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E111" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
@@ -2947,6 +3245,9 @@
       <c r="D112" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E112" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
@@ -2961,6 +3262,9 @@
       <c r="D113" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E113" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
@@ -2975,6 +3279,9 @@
       <c r="D114" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E114" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
@@ -2989,6 +3296,9 @@
       <c r="D115" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E115" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
@@ -3003,6 +3313,9 @@
       <c r="D116" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E116" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
@@ -3017,6 +3330,9 @@
       <c r="D117" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E117" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
@@ -3031,6 +3347,9 @@
       <c r="D118" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E118" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
@@ -3045,6 +3364,9 @@
       <c r="D119" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E119" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
@@ -3059,6 +3381,9 @@
       <c r="D120" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E120" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
@@ -3073,6 +3398,9 @@
       <c r="D121" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E121" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
@@ -3087,6 +3415,9 @@
       <c r="D122" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E122" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
@@ -3101,6 +3432,9 @@
       <c r="D123" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E123" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
@@ -3115,6 +3449,9 @@
       <c r="D124" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E124" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
@@ -3129,6 +3466,9 @@
       <c r="D125" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E125" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
@@ -3143,6 +3483,9 @@
       <c r="D126" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E126" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
@@ -3157,6 +3500,9 @@
       <c r="D127" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E127" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
@@ -3171,6 +3517,9 @@
       <c r="D128" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E128" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
@@ -3185,6 +3534,9 @@
       <c r="D129" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E129" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
@@ -3199,6 +3551,9 @@
       <c r="D130" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E130" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
@@ -3213,6 +3568,9 @@
       <c r="D131" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E131" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
@@ -3227,6 +3585,9 @@
       <c r="D132" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E132" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
@@ -3241,6 +3602,9 @@
       <c r="D133" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E133" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
@@ -3255,6 +3619,9 @@
       <c r="D134" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E134" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
@@ -3269,6 +3636,9 @@
       <c r="D135" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E135" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
@@ -3283,6 +3653,9 @@
       <c r="D136" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E136" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
@@ -3297,6 +3670,9 @@
       <c r="D137" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E137" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
@@ -3311,6 +3687,9 @@
       <c r="D138" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E138" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
@@ -3325,6 +3704,9 @@
       <c r="D139" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E139" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
@@ -3339,6 +3721,9 @@
       <c r="D140" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E140" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
@@ -3353,6 +3738,9 @@
       <c r="D141" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E141" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
@@ -3367,6 +3755,9 @@
       <c r="D142" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E142" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
@@ -3381,6 +3772,9 @@
       <c r="D143" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E143" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
@@ -3395,6 +3789,9 @@
       <c r="D144" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E144" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
@@ -3409,6 +3806,9 @@
       <c r="D145" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E145" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
@@ -3423,6 +3823,9 @@
       <c r="D146" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E146" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
@@ -3437,6 +3840,9 @@
       <c r="D147" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E147" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
@@ -3451,6 +3857,9 @@
       <c r="D148" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E148" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
@@ -3465,6 +3874,9 @@
       <c r="D149" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E149" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
@@ -3479,6 +3891,9 @@
       <c r="D150" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E150" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
@@ -3493,6 +3908,9 @@
       <c r="D151" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E151" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
@@ -3507,6 +3925,9 @@
       <c r="D152" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E152" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
@@ -3521,6 +3942,9 @@
       <c r="D153" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E153" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
@@ -3535,6 +3959,9 @@
       <c r="D154" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E154" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
@@ -3549,6 +3976,9 @@
       <c r="D155" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E155" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
@@ -3563,6 +3993,9 @@
       <c r="D156" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E156" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
@@ -3577,6 +4010,9 @@
       <c r="D157" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E157" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
@@ -3591,6 +4027,9 @@
       <c r="D158" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E158" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
@@ -3605,6 +4044,9 @@
       <c r="D159" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E159" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
@@ -3619,6 +4061,9 @@
       <c r="D160" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E160" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
@@ -3633,6 +4078,9 @@
       <c r="D161" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E161" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
@@ -3647,6 +4095,9 @@
       <c r="D162" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E162" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
@@ -3661,6 +4112,9 @@
       <c r="D163" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E163" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
@@ -3675,6 +4129,9 @@
       <c r="D164" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E164" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
@@ -3689,6 +4146,9 @@
       <c r="D165" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E165" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
@@ -3703,6 +4163,9 @@
       <c r="D166" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E166" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
@@ -3717,6 +4180,9 @@
       <c r="D167" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E167" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
@@ -3731,6 +4197,9 @@
       <c r="D168" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E168" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
@@ -3745,6 +4214,9 @@
       <c r="D169" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E169" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
@@ -3759,6 +4231,9 @@
       <c r="D170" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E170" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
@@ -3773,6 +4248,9 @@
       <c r="D171" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E171" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
@@ -3787,6 +4265,9 @@
       <c r="D172" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E172" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="s">
@@ -3801,6 +4282,9 @@
       <c r="D173" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E173" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="s">
@@ -3815,6 +4299,9 @@
       <c r="D174" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E174" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
@@ -3829,6 +4316,9 @@
       <c r="D175" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E175" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
@@ -3843,6 +4333,9 @@
       <c r="D176" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E176" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
@@ -3857,6 +4350,9 @@
       <c r="D177" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E177" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
@@ -3871,6 +4367,9 @@
       <c r="D178" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E178" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
@@ -3885,6 +4384,9 @@
       <c r="D179" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E179" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
@@ -3899,6 +4401,9 @@
       <c r="D180" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E180" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
@@ -3913,6 +4418,9 @@
       <c r="D181" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E181" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
@@ -3927,6 +4435,9 @@
       <c r="D182" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E182" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
@@ -3941,6 +4452,9 @@
       <c r="D183" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E183" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
@@ -3955,6 +4469,9 @@
       <c r="D184" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E184" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
@@ -3969,6 +4486,9 @@
       <c r="D185" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E185" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
@@ -3983,6 +4503,9 @@
       <c r="D186" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E186" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
@@ -3997,6 +4520,9 @@
       <c r="D187" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E187" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
@@ -4011,6 +4537,9 @@
       <c r="D188" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E188" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
@@ -4025,6 +4554,9 @@
       <c r="D189" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E189" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
@@ -4039,6 +4571,9 @@
       <c r="D190" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E190" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
@@ -4053,6 +4588,9 @@
       <c r="D191" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E191" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
@@ -4067,6 +4605,9 @@
       <c r="D192" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E192" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="s">
@@ -4081,6 +4622,9 @@
       <c r="D193" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E193" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
@@ -4095,6 +4639,9 @@
       <c r="D194" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E194" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
@@ -4109,6 +4656,9 @@
       <c r="D195" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E195" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
@@ -4123,6 +4673,9 @@
       <c r="D196" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E196" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
@@ -4137,6 +4690,9 @@
       <c r="D197" s="1" t="n">
         <v>132.7</v>
       </c>
+      <c r="E197" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
@@ -4151,6 +4707,9 @@
       <c r="D198" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E198" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
@@ -4165,6 +4724,9 @@
       <c r="D199" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E199" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="s">
@@ -4179,6 +4741,9 @@
       <c r="D200" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E200" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
@@ -4193,6 +4758,9 @@
       <c r="D201" s="1" t="n">
         <v>132.7</v>
       </c>
+      <c r="E201" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="s">
@@ -4207,6 +4775,9 @@
       <c r="D202" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E202" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="s">
@@ -4221,6 +4792,9 @@
       <c r="D203" s="1" t="n">
         <v>132.66</v>
       </c>
+      <c r="E203" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="s">
@@ -4235,6 +4809,9 @@
       <c r="D204" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E204" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
@@ -4249,6 +4826,9 @@
       <c r="D205" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E205" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
@@ -4263,6 +4843,9 @@
       <c r="D206" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E206" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
@@ -4277,6 +4860,9 @@
       <c r="D207" s="1" t="n">
         <v>132.66</v>
       </c>
+      <c r="E207" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
@@ -4291,6 +4877,9 @@
       <c r="D208" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E208" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
@@ -4305,6 +4894,9 @@
       <c r="D209" s="1" t="s">
         <v>239</v>
       </c>
+      <c r="E209" s="1" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
@@ -4319,6 +4911,9 @@
       <c r="D210" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E210" s="1" t="n">
+        <v>103.2</v>
+      </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
@@ -4333,6 +4928,9 @@
       <c r="D211" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E211" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
@@ -4347,6 +4945,9 @@
       <c r="D212" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E212" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
@@ -4361,6 +4962,9 @@
       <c r="D213" s="1" t="n">
         <v>385</v>
       </c>
+      <c r="E213" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="s">
@@ -4375,6 +4979,9 @@
       <c r="D214" s="1" t="n">
         <v>385</v>
       </c>
+      <c r="E214" s="1" t="n">
+        <v>103.2</v>
+      </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="s">
@@ -4389,6 +4996,9 @@
       <c r="D215" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E215" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
@@ -4403,6 +5013,9 @@
       <c r="D216" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E216" s="1" t="n">
+        <v>109.8</v>
+      </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
@@ -4417,6 +5030,9 @@
       <c r="D217" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E217" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="s">
@@ -4431,6 +5047,9 @@
       <c r="D218" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E218" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="s">
@@ -4445,6 +5064,9 @@
       <c r="D219" s="1" t="n">
         <v>437.9</v>
       </c>
+      <c r="E219" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="s">
@@ -4459,6 +5081,9 @@
       <c r="D220" s="1" t="n">
         <v>437.9</v>
       </c>
+      <c r="E220" s="1" t="n">
+        <v>109.8</v>
+      </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="s">
@@ -4473,6 +5098,9 @@
       <c r="D221" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E221" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="s">
@@ -4487,6 +5115,9 @@
       <c r="D222" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E222" s="1" t="n">
+        <v>61.9</v>
+      </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="s">
@@ -4501,6 +5132,9 @@
       <c r="D223" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E223" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="s">
@@ -4515,6 +5149,9 @@
       <c r="D224" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E224" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="s">
@@ -4529,6 +5166,9 @@
       <c r="D225" s="1" t="n">
         <v>141</v>
       </c>
+      <c r="E225" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="s">
@@ -4543,6 +5183,9 @@
       <c r="D226" s="1" t="n">
         <v>141</v>
       </c>
+      <c r="E226" s="1" t="n">
+        <v>61.9</v>
+      </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="s">
@@ -4557,6 +5200,9 @@
       <c r="D227" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E227" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="s">
@@ -4571,6 +5217,9 @@
       <c r="D228" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E228" s="1" t="n">
+        <v>78.4</v>
+      </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="s">
@@ -4585,6 +5234,9 @@
       <c r="D229" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E229" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
@@ -4599,6 +5251,9 @@
       <c r="D230" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E230" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
@@ -4613,6 +5268,9 @@
       <c r="D231" s="1" t="n">
         <v>99.9</v>
       </c>
+      <c r="E231" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="s">
@@ -4627,6 +5285,9 @@
       <c r="D232" s="1" t="n">
         <v>99.9</v>
       </c>
+      <c r="E232" s="1" t="n">
+        <v>78.4</v>
+      </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="s">
@@ -4641,6 +5302,9 @@
       <c r="D233" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E233" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="s">
@@ -4655,6 +5319,9 @@
       <c r="D234" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E234" s="1" t="n">
+        <v>64.3</v>
+      </c>
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="s">
@@ -4669,6 +5336,9 @@
       <c r="D235" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E235" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="s">
@@ -4683,6 +5353,9 @@
       <c r="D236" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E236" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="s">
@@ -4697,6 +5370,9 @@
       <c r="D237" s="1" t="n">
         <v>89</v>
       </c>
+      <c r="E237" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="s">
@@ -4711,6 +5387,9 @@
       <c r="D238" s="1" t="n">
         <v>89</v>
       </c>
+      <c r="E238" s="1" t="n">
+        <v>64.3</v>
+      </c>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="s">
@@ -4725,6 +5404,9 @@
       <c r="D239" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E239" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="s">
@@ -4739,6 +5421,9 @@
       <c r="D240" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E240" s="1" t="n">
+        <v>165</v>
+      </c>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="s">
@@ -4753,6 +5438,9 @@
       <c r="D241" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E241" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="s">
@@ -4767,6 +5455,9 @@
       <c r="D242" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E242" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="s">
@@ -4781,6 +5472,9 @@
       <c r="D243" s="1" t="n">
         <v>11.7</v>
       </c>
+      <c r="E243" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="244" s="5" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A244" s="5" t="s">
@@ -4794,6 +5488,9 @@
       </c>
       <c r="D244" s="5" t="n">
         <v>11.7</v>
+      </c>
+      <c r="E244" s="5" t="n">
+        <v>165</v>
       </c>
       <c r="ALB244" s="1"/>
       <c r="ALC244" s="1"/>
@@ -4844,6 +5541,9 @@
       <c r="D245" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E245" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="s">
@@ -4858,6 +5558,9 @@
       <c r="D246" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E246" s="1" t="n">
+        <v>1053.4</v>
+      </c>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="s">
@@ -4872,6 +5575,9 @@
       <c r="D247" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E247" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
@@ -4886,6 +5592,9 @@
       <c r="D248" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E248" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="s">
@@ -4897,6 +5606,9 @@
       <c r="C249" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E249" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="s">
@@ -4911,6 +5623,9 @@
       <c r="D250" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E250" s="1" t="n">
+        <v>1053.4</v>
+      </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A251" s="1" t="s">
@@ -4925,6 +5640,9 @@
       <c r="D251" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E251" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="s">
@@ -4939,6 +5657,9 @@
       <c r="D252" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E252" s="1" t="n">
+        <v>216.1</v>
+      </c>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A253" s="1" t="s">
@@ -4953,6 +5674,9 @@
       <c r="D253" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E253" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A254" s="1" t="s">
@@ -4967,6 +5691,9 @@
       <c r="D254" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E254" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A255" s="1" t="s">
@@ -4978,6 +5705,9 @@
       <c r="C255" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E255" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A256" s="1" t="s">
@@ -4992,6 +5722,9 @@
       <c r="D256" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E256" s="1" t="n">
+        <v>216.1</v>
+      </c>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="s">
@@ -5006,6 +5739,9 @@
       <c r="D257" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E257" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A258" s="1" t="s">
@@ -5020,6 +5756,9 @@
       <c r="D258" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E258" s="1" t="n">
+        <v>778.3</v>
+      </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="s">
@@ -5034,6 +5773,9 @@
       <c r="D259" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E259" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="s">
@@ -5048,6 +5790,9 @@
       <c r="D260" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E260" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="s">
@@ -5062,6 +5807,9 @@
       <c r="D261" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E261" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="s">
@@ -5076,6 +5824,9 @@
       <c r="D262" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E262" s="1" t="n">
+        <v>778.3</v>
+      </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="s">
@@ -5090,6 +5841,9 @@
       <c r="D263" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E263" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="s">
@@ -5104,6 +5858,9 @@
       <c r="D264" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E264" s="1" t="n">
+        <v>323.95</v>
+      </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="s">
@@ -5118,6 +5875,9 @@
       <c r="D265" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E265" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="s">
@@ -5132,6 +5892,9 @@
       <c r="D266" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E266" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="s">
@@ -5143,6 +5906,9 @@
       <c r="C267" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E267" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="s">
@@ -5157,6 +5923,9 @@
       <c r="D268" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E268" s="1" t="n">
+        <v>323.95</v>
+      </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="s">
@@ -5171,6 +5940,9 @@
       <c r="D269" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E269" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="s">
@@ -5185,6 +5957,9 @@
       <c r="D270" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E270" s="1" t="n">
+        <v>778.3</v>
+      </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A271" s="1" t="s">
@@ -5199,6 +5974,9 @@
       <c r="D271" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E271" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="s">
@@ -5213,6 +5991,9 @@
       <c r="D272" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E272" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="s">
@@ -5227,6 +6008,9 @@
       <c r="D273" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E273" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="s">
@@ -5241,6 +6025,9 @@
       <c r="D274" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E274" s="1" t="n">
+        <v>778.3</v>
+      </c>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="s">
@@ -5255,6 +6042,9 @@
       <c r="D275" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E275" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="s">
@@ -5269,6 +6059,9 @@
       <c r="D276" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E276" s="1" t="n">
+        <v>825.71</v>
+      </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="s">
@@ -5283,6 +6076,9 @@
       <c r="D277" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E277" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
@@ -5297,6 +6093,9 @@
       <c r="D278" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E278" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="s">
@@ -5308,6 +6107,9 @@
       <c r="C279" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E279" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="s">
@@ -5322,6 +6124,9 @@
       <c r="D280" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E280" s="1" t="n">
+        <v>825.71</v>
+      </c>
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A281" s="1" t="s">
@@ -5336,6 +6141,9 @@
       <c r="D281" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E281" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="s">
@@ -5350,6 +6158,9 @@
       <c r="D282" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E282" s="1" t="n">
+        <v>778.3</v>
+      </c>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="s">
@@ -5364,6 +6175,9 @@
       <c r="D283" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E283" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="s">
@@ -5378,6 +6192,9 @@
       <c r="D284" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E284" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="s">
@@ -5392,6 +6209,9 @@
       <c r="D285" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E285" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="s">
@@ -5406,6 +6226,9 @@
       <c r="D286" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E286" s="1" t="n">
+        <v>778.3</v>
+      </c>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="s">
@@ -5420,6 +6243,9 @@
       <c r="D287" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E287" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="s">
@@ -5434,6 +6260,9 @@
       <c r="D288" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E288" s="1" t="n">
+        <v>909.19</v>
+      </c>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="s">
@@ -5448,6 +6277,9 @@
       <c r="D289" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E289" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="s">
@@ -5462,6 +6294,9 @@
       <c r="D290" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E290" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="s">
@@ -5473,6 +6308,9 @@
       <c r="C291" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E291" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A292" s="1" t="s">
@@ -5487,6 +6325,9 @@
       <c r="D292" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E292" s="1" t="n">
+        <v>909.19</v>
+      </c>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="s">
@@ -5501,6 +6342,9 @@
       <c r="D293" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E293" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="s">
@@ -5515,6 +6359,9 @@
       <c r="D294" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E294" s="1" t="n">
+        <v>778.3</v>
+      </c>
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A295" s="1" t="s">
@@ -5529,6 +6376,9 @@
       <c r="D295" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E295" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A296" s="1" t="s">
@@ -5543,6 +6393,9 @@
       <c r="D296" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E296" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A297" s="1" t="s">
@@ -5557,6 +6410,9 @@
       <c r="D297" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E297" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A298" s="1" t="s">
@@ -5571,6 +6427,9 @@
       <c r="D298" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E298" s="1" t="n">
+        <v>778.3</v>
+      </c>
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="s">
@@ -5585,6 +6444,9 @@
       <c r="D299" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E299" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="s">
@@ -5599,6 +6461,9 @@
       <c r="D300" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E300" s="1" t="n">
+        <v>1216.59</v>
+      </c>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A301" s="1" t="s">
@@ -5613,6 +6478,9 @@
       <c r="D301" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E301" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A302" s="1" t="s">
@@ -5627,6 +6495,9 @@
       <c r="D302" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E302" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="s">
@@ -5641,6 +6512,9 @@
       <c r="D303" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E303" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="s">
@@ -5655,6 +6529,9 @@
       <c r="D304" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E304" s="1" t="n">
+        <v>1216.59</v>
+      </c>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A305" s="1" t="s">
@@ -5669,6 +6546,9 @@
       <c r="D305" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E305" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="s">
@@ -5683,6 +6563,9 @@
       <c r="D306" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E306" s="1" t="n">
+        <v>252.8</v>
+      </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A307" s="1" t="s">
@@ -5697,6 +6580,9 @@
       <c r="D307" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E307" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A308" s="1" t="s">
@@ -5711,6 +6597,9 @@
       <c r="D308" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E308" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A309" s="1" t="s">
@@ -5725,6 +6614,9 @@
       <c r="D309" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E309" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A310" s="1" t="s">
@@ -5739,6 +6631,9 @@
       <c r="D310" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E310" s="1" t="n">
+        <v>252.8</v>
+      </c>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="s">
@@ -5753,6 +6648,9 @@
       <c r="D311" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E311" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A312" s="1" t="s">
@@ -5767,6 +6665,9 @@
       <c r="D312" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E312" s="1" t="n">
+        <v>1141.08</v>
+      </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A313" s="1" t="s">
@@ -5781,6 +6682,9 @@
       <c r="D313" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E313" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A314" s="1" t="s">
@@ -5795,6 +6699,9 @@
       <c r="D314" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E314" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A315" s="1" t="s">
@@ -5809,6 +6716,9 @@
       <c r="D315" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E315" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A316" s="1" t="s">
@@ -5823,6 +6733,9 @@
       <c r="D316" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E316" s="1" t="n">
+        <v>1141.08</v>
+      </c>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A317" s="1" t="s">
@@ -5837,6 +6750,9 @@
       <c r="D317" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E317" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A318" s="1" t="s">
@@ -5851,6 +6767,9 @@
       <c r="D318" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E318" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A319" s="1" t="s">
@@ -5865,6 +6784,9 @@
       <c r="D319" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E319" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="s">
@@ -5879,6 +6801,9 @@
       <c r="D320" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E320" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A321" s="1" t="s">
@@ -5893,6 +6818,9 @@
       <c r="D321" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E321" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A322" s="1" t="s">
@@ -5907,6 +6835,9 @@
       <c r="D322" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E322" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A323" s="1" t="s">
@@ -5921,6 +6852,9 @@
       <c r="D323" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E323" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A324" s="1" t="s">
@@ -5935,6 +6869,9 @@
       <c r="D324" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E324" s="1" t="n">
+        <v>706.25</v>
+      </c>
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A325" s="1" t="s">
@@ -5949,6 +6886,9 @@
       <c r="D325" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E325" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A326" s="1" t="s">
@@ -5963,6 +6903,9 @@
       <c r="D326" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E326" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A327" s="1" t="s">
@@ -5977,6 +6920,9 @@
       <c r="D327" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E327" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A328" s="1" t="s">
@@ -5991,6 +6937,9 @@
       <c r="D328" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E328" s="1" t="n">
+        <v>706.25</v>
+      </c>
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A329" s="1" t="s">
@@ -6005,6 +6954,9 @@
       <c r="D329" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E329" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A330" s="1" t="s">
@@ -6019,6 +6971,9 @@
       <c r="D330" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E330" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A331" s="1" t="s">
@@ -6033,6 +6988,9 @@
       <c r="D331" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E331" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A332" s="1" t="s">
@@ -6047,6 +7005,9 @@
       <c r="D332" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E332" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A333" s="1" t="s">
@@ -6061,6 +7022,9 @@
       <c r="D333" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E333" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A334" s="1" t="s">
@@ -6075,6 +7039,9 @@
       <c r="D334" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E334" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="335" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A335" s="1" t="s">
@@ -6089,6 +7056,9 @@
       <c r="D335" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E335" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A336" s="1" t="s">
@@ -6103,6 +7073,9 @@
       <c r="D336" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E336" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A337" s="1" t="s">
@@ -6117,6 +7090,9 @@
       <c r="D337" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E337" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="338" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A338" s="1" t="s">
@@ -6131,6 +7107,9 @@
       <c r="D338" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E338" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A339" s="1" t="s">
@@ -6145,6 +7124,9 @@
       <c r="D339" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E339" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="340" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A340" s="1" t="s">
@@ -6159,6 +7141,9 @@
       <c r="D340" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E340" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A341" s="1" t="s">
@@ -6173,6 +7158,9 @@
       <c r="D341" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E341" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="342" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A342" s="1" t="s">
@@ -6187,6 +7175,9 @@
       <c r="D342" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E342" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="343" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A343" s="1" t="s">
@@ -6201,6 +7192,9 @@
       <c r="D343" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E343" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="344" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A344" s="1" t="s">
@@ -6215,6 +7209,9 @@
       <c r="D344" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E344" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="345" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A345" s="1" t="s">
@@ -6229,6 +7226,9 @@
       <c r="D345" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E345" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="346" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A346" s="1" t="s">
@@ -6243,6 +7243,9 @@
       <c r="D346" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E346" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="347" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A347" s="1" t="s">
@@ -6257,6 +7260,9 @@
       <c r="D347" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E347" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="348" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A348" s="1" t="s">
@@ -6271,6 +7277,9 @@
       <c r="D348" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E348" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="349" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A349" s="1" t="s">
@@ -6285,6 +7294,9 @@
       <c r="D349" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E349" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="350" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A350" s="1" t="s">
@@ -6299,6 +7311,9 @@
       <c r="D350" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E350" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="351" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A351" s="6" t="s">
@@ -6313,6 +7328,9 @@
       <c r="D351" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E351" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="352" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A352" s="1" t="s">
@@ -6327,6 +7345,9 @@
       <c r="D352" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E352" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="353" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A353" s="6" t="s">
@@ -6341,6 +7362,9 @@
       <c r="D353" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E353" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="354" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A354" s="1" t="s">
@@ -6355,6 +7379,9 @@
       <c r="D354" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E354" s="1" t="n">
+        <v>4648.8</v>
+      </c>
     </row>
     <row r="355" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A355" s="1" t="s">
@@ -6369,6 +7396,9 @@
       <c r="D355" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E355" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="356" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A356" s="1" t="s">
@@ -6383,6 +7413,9 @@
       <c r="D356" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E356" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="357" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A357" s="1" t="s">
@@ -6397,6 +7430,9 @@
       <c r="D357" s="1" t="n">
         <v>615</v>
       </c>
+      <c r="E357" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="358" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A358" s="1" t="s">
@@ -6411,6 +7447,9 @@
       <c r="D358" s="1" t="n">
         <v>615</v>
       </c>
+      <c r="E358" s="1" t="n">
+        <v>4648.8</v>
+      </c>
     </row>
     <row r="359" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A359" s="1" t="s">
@@ -6425,6 +7464,9 @@
       <c r="D359" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E359" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="360" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A360" s="1" t="s">
@@ -6439,6 +7481,9 @@
       <c r="D360" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E360" s="1" t="n">
+        <v>5692.07</v>
+      </c>
     </row>
     <row r="361" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A361" s="1" t="s">
@@ -6453,6 +7498,9 @@
       <c r="D361" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E361" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="362" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A362" s="1" t="s">
@@ -6467,6 +7515,9 @@
       <c r="D362" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E362" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="363" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A363" s="1" t="s">
@@ -6481,6 +7532,9 @@
       <c r="D363" s="1" t="n">
         <v>549.5</v>
       </c>
+      <c r="E363" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="364" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A364" s="1" t="s">
@@ -6495,6 +7549,9 @@
       <c r="D364" s="1" t="n">
         <v>549.5</v>
       </c>
+      <c r="E364" s="1" t="n">
+        <v>5692.07</v>
+      </c>
     </row>
     <row r="365" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A365" s="1" t="s">
@@ -6509,6 +7566,9 @@
       <c r="D365" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E365" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="366" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A366" s="1" t="s">
@@ -6523,6 +7583,9 @@
       <c r="D366" s="1" t="s">
         <v>399</v>
       </c>
+      <c r="E366" s="1" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="367" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A367" s="7" t="s">
@@ -6537,6 +7600,9 @@
       <c r="D367" s="2" t="s">
         <v>403</v>
       </c>
+      <c r="E367" s="2" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="368" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A368" s="1" t="s">
@@ -6551,6 +7617,9 @@
       <c r="D368" s="2" t="n">
         <v>1172</v>
       </c>
+      <c r="E368" s="2" t="n">
+        <v>2952</v>
+      </c>
     </row>
     <row r="369" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A369" s="1" t="s">
@@ -6565,6 +7634,9 @@
       <c r="D369" s="2" t="n">
         <v>738.36</v>
       </c>
+      <c r="E369" s="2" t="n">
+        <v>4487</v>
+      </c>
     </row>
     <row r="370" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A370" s="8" t="s">
@@ -6573,8 +7645,9 @@
       <c r="B370" s="8"/>
       <c r="C370" s="8"/>
       <c r="D370" s="8" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E370" s="8"/>
     </row>
     <row r="371" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A371" s="8" t="s">
@@ -6583,8 +7656,9 @@
       <c r="B371" s="8"/>
       <c r="C371" s="8"/>
       <c r="D371" s="8" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E371" s="8"/>
     </row>
     <row r="372" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A372" s="8" t="s">
@@ -6593,8 +7667,9 @@
       <c r="B372" s="8"/>
       <c r="C372" s="8"/>
       <c r="D372" s="8" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E372" s="8"/>
     </row>
     <row r="373" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A373" s="9" t="s">
@@ -6603,8 +7678,9 @@
       <c r="B373" s="8"/>
       <c r="C373" s="8"/>
       <c r="D373" s="8" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E373" s="8"/>
     </row>
     <row r="374" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A374" s="9" t="s">
@@ -6612,10 +7688,13 @@
       </c>
       <c r="B374" s="8"/>
       <c r="C374" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D374" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="E374" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6625,8 +7704,9 @@
       <c r="B375" s="8"/>
       <c r="C375" s="8"/>
       <c r="D375" s="8" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E375" s="8"/>
     </row>
     <row r="376" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A376" s="6" t="s">
@@ -6635,8 +7715,9 @@
       <c r="B376" s="8"/>
       <c r="C376" s="8"/>
       <c r="D376" s="8" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E376" s="8"/>
     </row>
     <row r="377" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A377" s="6" t="s">
@@ -6645,8 +7726,9 @@
       <c r="B377" s="8"/>
       <c r="C377" s="8"/>
       <c r="D377" s="8" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E377" s="8"/>
     </row>
     <row r="378" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A378" s="6" t="s">
@@ -6655,8 +7737,9 @@
       <c r="B378" s="8"/>
       <c r="C378" s="8"/>
       <c r="D378" s="8" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E378" s="8"/>
     </row>
     <row r="379" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A379" s="7" t="s">
@@ -6670,6 +7753,9 @@
       </c>
       <c r="D379" s="7" t="n">
         <v>63.02</v>
+      </c>
+      <c r="E379" s="7" t="n">
+        <v>0</v>
       </c>
       <c r="ALB379" s="1"/>
       <c r="ALC379" s="1"/>
@@ -6719,6 +7805,9 @@
       </c>
       <c r="D380" s="7" t="n">
         <v>437.9</v>
+      </c>
+      <c r="E380" s="7" t="n">
+        <v>109.8</v>
       </c>
       <c r="ALB380" s="1"/>
       <c r="ALC380" s="1"/>

</xml_diff>

<commit_message>
add non-gov profile to get_cost_totals_project() and total_costs_benefits_bar_chart(). all test passing. these changes required changes to keys in real master data
</commit_message>
<xml_diff>
--- a/tests/resources/cost_test_master_4_2018.xlsx
+++ b/tests/resources/cost_test_master_4_2018.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="417">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -760,7 +760,7 @@
     <t xml:space="preserve">Pre 18-19 BL Income both Revenue and Capital</t>
   </si>
   <si>
-    <t xml:space="preserve">Pre 18-19 CDEL Forecast Total</t>
+    <t xml:space="preserve">Pre-profile CDEL</t>
   </si>
   <si>
     <t xml:space="preserve">Pre 18-19 CDEL Forecast recurring new costs</t>
@@ -769,7 +769,7 @@
     <t xml:space="preserve">Pre 18-19 CDEL Forecast recurring old costs</t>
   </si>
   <si>
-    <t xml:space="preserve">Pre 18-19 Forecast Non-Gov</t>
+    <t xml:space="preserve">Pre-profile non-gov</t>
   </si>
   <si>
     <t xml:space="preserve">Pre 18-19 CDEL Forecast Total WLC</t>
@@ -1268,9 +1268,6 @@
   </si>
   <si>
     <t xml:space="preserve">Pre-profile RDEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pre-profile CDEL</t>
   </si>
   <si>
     <t xml:space="preserve">Re-baseline this quarter</t>
@@ -1324,14 +1321,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFC9211E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFC9211E"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1414,11 +1411,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1518,11 +1515,11 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B358" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B338" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A358" activeCellId="0" sqref="A358"/>
-      <selection pane="bottomRight" activeCell="G369" activeCellId="0" sqref="G369"/>
+      <selection pane="bottomLeft" activeCell="A338" activeCellId="0" sqref="A338"/>
+      <selection pane="bottomRight" activeCell="A351" activeCellId="0" sqref="A351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5001,7 +4998,7 @@
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A216" s="1" t="s">
+      <c r="A216" s="5" t="s">
         <v>246</v>
       </c>
       <c r="B216" s="1" t="n">
@@ -5052,7 +5049,7 @@
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A219" s="1" t="s">
+      <c r="A219" s="5" t="s">
         <v>249</v>
       </c>
       <c r="B219" s="1" t="n">
@@ -5476,20 +5473,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" s="5" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A244" s="5" t="s">
+    <row r="244" s="6" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A244" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="B244" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C244" s="5" t="n">
+      <c r="B244" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C244" s="6" t="n">
         <v>165</v>
       </c>
-      <c r="D244" s="5" t="n">
+      <c r="D244" s="6" t="n">
         <v>11.7</v>
       </c>
-      <c r="E244" s="5" t="n">
+      <c r="E244" s="6" t="n">
         <v>165</v>
       </c>
       <c r="ALB244" s="1"/>
@@ -7316,7 +7313,7 @@
       </c>
     </row>
     <row r="351" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A351" s="6" t="s">
+      <c r="A351" s="7" t="s">
         <v>381</v>
       </c>
       <c r="B351" s="1" t="n">
@@ -7350,7 +7347,7 @@
       </c>
     </row>
     <row r="353" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A353" s="6" t="s">
+      <c r="A353" s="7" t="s">
         <v>383</v>
       </c>
       <c r="B353" s="1" t="n">
@@ -7588,7 +7585,7 @@
       </c>
     </row>
     <row r="367" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A367" s="7" t="s">
+      <c r="A367" s="5" t="s">
         <v>400</v>
       </c>
       <c r="B367" s="2" t="s">
@@ -7709,7 +7706,7 @@
       <c r="E375" s="8"/>
     </row>
     <row r="376" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A376" s="6" t="s">
+      <c r="A376" s="7" t="s">
         <v>412</v>
       </c>
       <c r="B376" s="8"/>
@@ -7720,7 +7717,7 @@
       <c r="E376" s="8"/>
     </row>
     <row r="377" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A377" s="6" t="s">
+      <c r="A377" s="7" t="s">
         <v>413</v>
       </c>
       <c r="B377" s="8"/>
@@ -7731,7 +7728,7 @@
       <c r="E377" s="8"/>
     </row>
     <row r="378" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A378" s="6" t="s">
+      <c r="A378" s="7" t="s">
         <v>414</v>
       </c>
       <c r="B378" s="8"/>
@@ -7741,20 +7738,20 @@
       </c>
       <c r="E378" s="8"/>
     </row>
-    <row r="379" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A379" s="7" t="s">
+    <row r="379" s="5" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A379" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="B379" s="7" t="n">
+      <c r="B379" s="5" t="n">
         <v>62.07</v>
       </c>
-      <c r="C379" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D379" s="7" t="n">
+      <c r="C379" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D379" s="5" t="n">
         <v>63.02</v>
       </c>
-      <c r="E379" s="7" t="n">
+      <c r="E379" s="5" t="n">
         <v>0</v>
       </c>
       <c r="ALB379" s="1"/>
@@ -7793,63 +7790,12 @@
       <c r="AMI379" s="0"/>
       <c r="AMJ379" s="0"/>
     </row>
-    <row r="380" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A380" s="7" t="s">
+    <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A380" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="B380" s="7" t="n">
-        <v>583.73</v>
-      </c>
-      <c r="C380" s="7" t="n">
-        <v>109.8</v>
-      </c>
-      <c r="D380" s="7" t="n">
-        <v>437.9</v>
-      </c>
-      <c r="E380" s="7" t="n">
-        <v>109.8</v>
-      </c>
-      <c r="ALB380" s="1"/>
-      <c r="ALC380" s="1"/>
-      <c r="ALD380" s="1"/>
-      <c r="ALE380" s="1"/>
-      <c r="ALF380" s="1"/>
-      <c r="ALG380" s="1"/>
-      <c r="ALH380" s="1"/>
-      <c r="ALI380" s="1"/>
-      <c r="ALJ380" s="1"/>
-      <c r="ALK380" s="1"/>
-      <c r="ALL380" s="1"/>
-      <c r="ALM380" s="1"/>
-      <c r="ALN380" s="1"/>
-      <c r="ALO380" s="1"/>
-      <c r="ALP380" s="1"/>
-      <c r="ALQ380" s="1"/>
-      <c r="ALR380" s="1"/>
-      <c r="ALS380" s="1"/>
-      <c r="ALT380" s="1"/>
-      <c r="ALU380" s="1"/>
-      <c r="ALV380" s="1"/>
-      <c r="ALW380" s="1"/>
-      <c r="ALX380" s="1"/>
-      <c r="ALY380" s="1"/>
-      <c r="ALZ380" s="1"/>
-      <c r="AMA380" s="1"/>
-      <c r="AMB380" s="1"/>
-      <c r="AMC380" s="1"/>
-      <c r="AMD380" s="1"/>
-      <c r="AME380" s="1"/>
-      <c r="AMF380" s="1"/>
-      <c r="AMG380" s="1"/>
-      <c r="AMH380" s="1"/>
-      <c r="AMI380" s="0"/>
-      <c r="AMJ380" s="0"/>
-    </row>
-    <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A381" s="10" t="s">
-        <v>417</v>
-      </c>
-    </row>
+    </row>
+    <row r="1046945" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1046946" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1046947" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1046948" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
changes to cdel key names
</commit_message>
<xml_diff>
--- a/tests/resources/cost_test_master_4_2018.xlsx
+++ b/tests/resources/cost_test_master_4_2018.xlsx
@@ -4821,7 +4821,7 @@
     <row r="228" ht="15" customHeight="1" s="12">
       <c r="A228" s="11" t="inlineStr">
         <is>
-          <t>18-19 CDEL Forecast Total</t>
+          <t>18-19 CDEL Forecast one off new costs</t>
         </is>
       </c>
       <c r="B228" s="11" t="n">
@@ -5049,7 +5049,7 @@
     <row r="240" ht="15" customHeight="1" s="12">
       <c r="A240" s="11" t="inlineStr">
         <is>
-          <t>19-20 CDEL Forecast Total</t>
+          <t>19-20 CDEL Forecast one off new costs</t>
         </is>
       </c>
       <c r="B240" s="11" t="n">
@@ -5309,7 +5309,7 @@
     <row r="252" ht="15" customHeight="1" s="12">
       <c r="A252" s="11" t="inlineStr">
         <is>
-          <t>20-21 CDEL Forecast Total</t>
+          <t>20-21 CDEL Forecast one off new costs</t>
         </is>
       </c>
       <c r="B252" s="11" t="n">
@@ -5534,7 +5534,7 @@
     <row r="264" ht="15" customHeight="1" s="12">
       <c r="A264" s="11" t="inlineStr">
         <is>
-          <t>21-22 CDEL Forecast Total</t>
+          <t>21-22 CDEL Forecast one off new costs</t>
         </is>
       </c>
       <c r="B264" s="11" t="n">
@@ -5759,7 +5759,7 @@
     <row r="276" ht="15" customHeight="1" s="12">
       <c r="A276" s="11" t="inlineStr">
         <is>
-          <t>22-23 CDEL Forecast Total</t>
+          <t>22-23 CDEL Forecast one off new costs</t>
         </is>
       </c>
       <c r="B276" s="11" t="n">
@@ -5984,7 +5984,7 @@
     <row r="288" ht="15" customHeight="1" s="12">
       <c r="A288" s="11" t="inlineStr">
         <is>
-          <t>23-24 CDEL Forecast Total</t>
+          <t>23-24 CDEL Forecast one off new costs</t>
         </is>
       </c>
       <c r="B288" s="11" t="n">
@@ -6209,7 +6209,7 @@
     <row r="300" ht="15" customHeight="1" s="12">
       <c r="A300" s="11" t="inlineStr">
         <is>
-          <t>24-25 CDEL Forecast Total</t>
+          <t>24-25 CDEL Forecast one off new costs</t>
         </is>
       </c>
       <c r="B300" s="11" t="n">
@@ -6437,7 +6437,7 @@
     <row r="312" ht="15" customHeight="1" s="12">
       <c r="A312" s="11" t="inlineStr">
         <is>
-          <t>25-26 CDEL Forecast Total</t>
+          <t>25-26 CDEL Forecast one off new costs</t>
         </is>
       </c>
       <c r="B312" s="11" t="n">
@@ -6665,7 +6665,7 @@
     <row r="324" ht="15" customHeight="1" s="12">
       <c r="A324" s="11" t="inlineStr">
         <is>
-          <t>26-27 CDEL Forecast Total</t>
+          <t>26-27 CDEL Forecast one off new costs</t>
         </is>
       </c>
       <c r="B324" s="11" t="n">
@@ -6893,7 +6893,7 @@
     <row r="336" ht="15" customHeight="1" s="12">
       <c r="A336" s="11" t="inlineStr">
         <is>
-          <t>27-28 CDEL Forecast Total</t>
+          <t>27-28 CDEL Forecast one off new costs</t>
         </is>
       </c>
       <c r="B336" s="11" t="n">

</xml_diff>

<commit_message>
change to test data set to include older cost figures. 16-17 added to year list. change_cost_keys working but needs tidying and to be put into proper tests
</commit_message>
<xml_diff>
--- a/tests/resources/cost_test_master_4_2018.xlsx
+++ b/tests/resources/cost_test_master_4_2018.xlsx
@@ -475,7 +475,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AMJ380"/>
+  <dimension ref="A1:AMK380"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B338" activePane="bottomRight" state="frozen"/>
@@ -1602,7 +1602,7 @@
     <row r="59" ht="15" customHeight="1" s="12">
       <c r="A59" s="11" t="inlineStr">
         <is>
-          <t>Pre 18-19 RDEL Forecast one off new costs</t>
+          <t xml:space="preserve">Pre-profile RDEL Forecast one off new costs </t>
         </is>
       </c>
       <c r="B59" s="11" t="n">
@@ -1834,7 +1834,7 @@
         </is>
       </c>
       <c r="B71" s="11" t="n">
-        <v>1.08</v>
+        <v>37.88</v>
       </c>
       <c r="C71" s="11" t="n">
         <v>0</v>
@@ -1852,9 +1852,7 @@
           <t>18-19 RDEL Forecast recurring new costs</t>
         </is>
       </c>
-      <c r="B72" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="B72" s="11" t="n"/>
       <c r="C72" s="11" t="n">
         <v>0</v>
       </c>
@@ -1899,9 +1897,7 @@
       <c r="D74" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E74" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="E74" s="11" t="n"/>
     </row>
     <row r="75" ht="15" customHeight="1" s="12">
       <c r="A75" s="11" t="inlineStr">
@@ -1910,7 +1906,7 @@
         </is>
       </c>
       <c r="B75" s="11" t="n">
-        <v>1.08</v>
+        <v>37.88</v>
       </c>
       <c r="C75" s="11" t="n">
         <v>0</v>
@@ -1937,9 +1933,7 @@
       <c r="D76" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E76" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="E76" s="11" t="n"/>
     </row>
     <row r="77" ht="15" customHeight="1" s="12">
       <c r="A77" s="11" t="inlineStr">
@@ -2062,7 +2056,7 @@
         </is>
       </c>
       <c r="B83" s="11" t="n">
-        <v>2</v>
+        <v>34.49</v>
       </c>
       <c r="C83" s="11" t="n">
         <v>0</v>
@@ -2080,9 +2074,7 @@
           <t>19-20 RDEL Forecast recurring new costs</t>
         </is>
       </c>
-      <c r="B84" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="B84" s="11" t="n"/>
       <c r="C84" s="11" t="n">
         <v>0</v>
       </c>
@@ -2127,9 +2119,7 @@
       <c r="D86" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E86" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="E86" s="11" t="n"/>
     </row>
     <row r="87" ht="15" customHeight="1" s="12">
       <c r="A87" s="11" t="inlineStr">
@@ -2138,7 +2128,7 @@
         </is>
       </c>
       <c r="B87" s="11" t="n">
-        <v>2</v>
+        <v>34.49</v>
       </c>
       <c r="C87" s="11" t="n">
         <v>0</v>
@@ -2165,9 +2155,7 @@
       <c r="D88" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E88" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="E88" s="11" t="n"/>
     </row>
     <row r="89" ht="15" customHeight="1" s="12">
       <c r="A89" s="11" t="inlineStr">
@@ -4825,16 +4813,16 @@
         </is>
       </c>
       <c r="B228" s="11" t="n">
-        <v>14.25</v>
+        <v>25</v>
       </c>
       <c r="C228" s="11" t="n">
-        <v>78.40000000000001</v>
+        <v>61.9</v>
       </c>
       <c r="D228" s="11" t="n">
         <v>0</v>
       </c>
       <c r="E228" s="11" t="n">
-        <v>78.40000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="229" ht="15" customHeight="1" s="12">
@@ -4843,9 +4831,7 @@
           <t>18-19 CDEL Forecast recurring new costs</t>
         </is>
       </c>
-      <c r="B229" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="B229" s="11" t="n"/>
       <c r="C229" s="11" t="n">
         <v>0</v>
       </c>
@@ -4884,14 +4870,12 @@
       <c r="B231" s="11" t="n">
         <v>96</v>
       </c>
-      <c r="C231" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="C231" s="11" t="n"/>
       <c r="D231" s="11" t="n">
-        <v>99.90000000000001</v>
+        <v>71.09999999999999</v>
       </c>
       <c r="E231" s="11" t="n">
-        <v>0</v>
+        <v>66.09999999999999</v>
       </c>
     </row>
     <row r="232" ht="15" customHeight="1" s="12">
@@ -4909,9 +4893,7 @@
       <c r="D232" s="11" t="n">
         <v>99.90000000000001</v>
       </c>
-      <c r="E232" s="11" t="n">
-        <v>78.40000000000001</v>
-      </c>
+      <c r="E232" s="11" t="n"/>
     </row>
     <row r="233" ht="15" customHeight="1" s="12">
       <c r="A233" s="11" t="inlineStr">
@@ -4919,18 +4901,12 @@
           <t>18-19 Forecast - Income both Revenue and Capital</t>
         </is>
       </c>
-      <c r="B233" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C233" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="B233" s="11" t="n"/>
+      <c r="C233" s="11" t="n"/>
       <c r="D233" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E233" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="E233" s="11" t="n"/>
     </row>
     <row r="234" ht="15" customHeight="1" s="12">
       <c r="A234" s="11" t="inlineStr">
@@ -5056,13 +5032,13 @@
         <v>0</v>
       </c>
       <c r="C240" s="11" t="n">
-        <v>165</v>
+        <v>64.3</v>
       </c>
       <c r="D240" s="11" t="n">
         <v>0</v>
       </c>
       <c r="E240" s="11" t="n">
-        <v>165</v>
+        <v>0</v>
       </c>
     </row>
     <row r="241" ht="15" customHeight="1" s="12">
@@ -5109,17 +5085,15 @@
           <t>19-20 Forecast Non-Gov</t>
         </is>
       </c>
-      <c r="B243" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="B243" s="11" t="n"/>
       <c r="C243" s="11" t="n">
         <v>0</v>
       </c>
       <c r="D243" s="11" t="n">
-        <v>11.7</v>
+        <v>30.7</v>
       </c>
       <c r="E243" s="11" t="n">
-        <v>0</v>
+        <v>102.8</v>
       </c>
     </row>
     <row r="244" ht="15" customFormat="1" customHeight="1" s="17">
@@ -5138,7 +5112,7 @@
         <v>11.7</v>
       </c>
       <c r="E244" s="17" t="n">
-        <v>165</v>
+        <v>22.6</v>
       </c>
       <c r="ALB244" s="11" t="n"/>
       <c r="ALC244" s="11" t="n"/>
@@ -5182,18 +5156,12 @@
           <t>19-20 Forecast - Income both Revenue and Capital</t>
         </is>
       </c>
-      <c r="B245" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C245" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="B245" s="11" t="n"/>
+      <c r="C245" s="11" t="n"/>
       <c r="D245" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E245" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="E245" s="11" t="n"/>
     </row>
     <row r="246" ht="15" customHeight="1" s="12">
       <c r="A246" s="11" t="inlineStr">

</xml_diff>

<commit_message>
wp use of json data master
</commit_message>
<xml_diff>
--- a/tests/resources/cost_test_master_4_2018.xlsx
+++ b/tests/resources/cost_test_master_4_2018.xlsx
@@ -180,6 +180,74 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 

</xml_diff>